<commit_message>
three more comments to address
</commit_message>
<xml_diff>
--- a/Final Submission/comment_responses_update.xlsx
+++ b/Final Submission/comment_responses_update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gzuckerman/Documents/GitHub/Plasticity1/Final Submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9742AF70-8E8D-5447-908B-58FEDD9AA00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9650ED-9A92-EF4D-8F0A-658005B0E817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{5D8CA695-E3F1-9847-A2F9-D708B767974E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>The authors cite Arnold’s (2010) paper about informative parameters in AIC-based model selection, but then perform interpretation on models that contain uninformative parameters. My understanding is that the premise of Arnold (2010) is that if a nested model is within 2 AIC units of a more complex model, then the parameters in the more complex models are uninformative. Here, the authors identify parameters as “informative” when I believe the should not be; for example the top-ranked model in Appendix C contains no informative parameters, since the null model (with no covariates) is within 2 AIC units. </t>
   </si>
@@ -80,16 +80,6 @@
     <t>"Models having Di[DAIC] within about 0–2 units of the best model should be examined to see whether they differ from thebest model by 1 parameter and have essentially the same values of the maximized log-likelihood as the best model. In this case, the larger model is not really supported or competitive, but rather is ‘close’ only because it adds 1 parameter and therefore will be within 2Di units," from Arnold 2010</t>
   </si>
   <si>
-    <t>With the way that we performed model selection, whether or not a parameter is informative has nothing to do with how the model compares to the null model - instead it has to do with if the 85% CI overlaps zero. I think what the reviewer may be trying to get at is that there is a "penalty" for a model having more covariates, such that an extra covariate that is uninformative can still result in a model with 2AIC of the top model (see Note). Our top model had more than one parameter different from the next model, thus the fact that it was within 2AIC of the null model is irrelevant.
-We have clarified the text that we used the 85% CI not overlapping 0 as an indicator of a informative parameter. We also added parameter CI ranges in Appendix S3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While it is true that switches in tactics could not occur if there were not multiple tactics present (ie migratory diversity), it is our understanding that an independent variable (ie herd diversity) being correlated to the dependent variable (switching) does not cause adverse effects in the modeling process. </t>
-  </si>
-  <si>
-    <t>Found a correlation between switching and herd migratory diversity of 0.21</t>
-  </si>
-  <si>
     <t>The variables are ssentially already time lagged since all variables are from the year before the switch occurs. It would certainly be interesting to see if years further back have impact on switching indicating a potential impact of memory, however that is out of scope of this analysis.</t>
   </si>
   <si>
@@ -97,15 +87,6 @@
   </si>
   <si>
     <t>The prediction column in Table 1 only uses the away from framing, saving for the social theme, in which we predict increased switching rates in all directions</t>
-  </si>
-  <si>
-    <t>added definition in text</t>
-  </si>
-  <si>
-    <t>reordered figure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As we stated in the last paragraph of the introduction, this is the largest sample of multiyear elk movement  data from the GYE ecosystem to answer this question. We added a sentence in the methods section clarifying the herd level representation covered by the dataset used in this report. </t>
   </si>
   <si>
     <t>We determined the switching "from" to be best suited to answering the question are elk switching from LDM tactics, which is important and many systems face decling long distance migrants. We initially sought to fit models for specific switches (ie resident to SDM, or resident to LDM) however our sample size was not large enough (mentioned in the second to last paragraph of the discussion section).</t>
@@ -119,46 +100,35 @@
     <t>We agree that our ability to speak about long-term trends of migratory behavior is limited. We mention this limitation in the second to last paragraph in the Discussion section, but have added to it in accordance with this comment. We have also made sure to specify that the trends we see are during our study period, and may or may not be reflected outside of it. If we do comment on the long term, we make sure to clearly state it is speculation rather than inference from the results</t>
   </si>
   <si>
-    <t>Does this appropirate convey the how much of the GYE our study covers?</t>
-  </si>
-  <si>
-    <t>created a new figure, though makes evident that many switches in tactic have relatively small magnitude, worried this might undermine the the work done. Not sure how to explain that what we have we have leabeled as biologically signifciant changes in behavior are actually pretty minor. On the other hand, we did claim that "switches" were more short-term adjustments</t>
-  </si>
-  <si>
-    <t>The correlation between switching prevalence and herd migratory diversity was only 0.21. Of the X herds we studied, X had more than 1 migratory strategy [reword to make the point that pretty much all the herds had at least 2 behaviors - i.e., could be more like 72% of the herds we studied (n = X out of X) had more than one migratory strategy present). In our opinion, if behavioral switching is an important driver of migratory changes, then an elk should be similarly likely to switch between 2 ta</t>
-  </si>
-  <si>
     <t>between 2 tactics as between 4 - i.e., the number of possible behavioral tactics matters less than the propensity to change between any tactic.</t>
   </si>
   <si>
     <t>2. you only need 2 strategies for switching, doesn't matter how many</t>
   </si>
   <si>
-    <t>1. mot of the herds had more than 1 strategy 2. you only need 2 strategies for switching, doesn't matter how many 3. 0.2 correlation low</t>
-  </si>
-  <si>
-    <t>We added a sentence in the methods section clarifying that this is the largest sample of multiyear elk movement data from the GYE ecosystem to answer this question.</t>
-  </si>
-  <si>
     <t>add this to disucssion: We note that although this is the most comprehensive sample of multiyear elk movement  data from the GYE ecosystem, it is possibleour results under- or oover-estimated switching rates given that we lacked multiple years of conescutive data from 6 of the 26 known herds in the ecosystem</t>
   </si>
   <si>
-    <t>double check this sentiment in the abstract</t>
-  </si>
-  <si>
-    <t>Thank you for making this suggestion. We have added a new figure (Fig. XXX) that visualizes the strength and direction of behavioral switches from each strategy. In addition to quantifying the specific amounts of change, the figure also shows that all stategies had switch events of relatively large proportions in addition to switches due to relatively smaller changes in elevation or distance.</t>
-  </si>
-  <si>
-    <t>[basically trying to say yes thre were some small changes, but there were also some big ones, and no strategy had conspicuously more or less of either - i.e. there are big elevation/distance differnces for each strategy in addition to the smaller ones)</t>
-  </si>
-  <si>
-    <t>add units to x and y axis</t>
-  </si>
-  <si>
     <t>could add sentence or two saying that bc of the automated nature of switching identification there could be elk that were in one year on one side of a cluster boundary and in the next, on the other. So there may be some switches that are not bioligically significant, relatively small differences. So we can't say whether all the switches we observed have considerable biolical consequences. We chose this automated apporach bc is it a repeatble objective way to classify behavior whitout predefining behaviors. It is possible that relatively minor shifts in distances traversed or elevation changed, its possibel that a switch may not have strogn bioligcal implications</t>
   </si>
   <si>
     <t>thank you we agree, we have added multiple sentences of discussion. We appreciate this concern as it important to note</t>
+  </si>
+  <si>
+    <t>With the way that we performed model selection, whether or not a parameter is informative is not related to how the model compares to the null model - instead it has to do with if the 85% CI overlaps zero. I think what the reviewer may be trying to get at is that there is a "penalty" for a model having more covariates, such that an extra covariate that is uninformative can still result in a model with 2AIC of the top model (see Note). Our top model had more than one parameter different from the next model, thus the fact that it was within 2AIC of the null model is irrelevant.
+We have clarified the text that we used the 85% CI not overlapping 0 as an indicator of a informative parameter. We also added parameter CI ranges in Appendix S3.</t>
+  </si>
+  <si>
+    <t>The correlation between switching prevalence and herd migratory diversity was only 0.21, which is quite low. Nearly all (90%) of the herds we studied had more than 1 migratory strategy. In our opinion, if behavioral switching is an important driver of migratory changes, then an elk should be similarly likely to switch between between 2 tactics as between 4 - i.e., the number of possible behavioral tactics matters less than the propensity to change between any tactic. Additionally, the diversity metric is not just a measure of the number of tactics, but the distribution within the herd as well, adding increased nuance to the relationship. With all the above factors considered, we believe there is still significant variation in the data that warrants the modeling we performed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for pointing out that we missed, this--it is a key point. We added a sentence in the methods section clarifying the herd level representation covered by the dataset used in this report. We also added a sentence in the discussion section about this as well. </t>
+  </si>
+  <si>
+    <t>This makes sense, we have reordered the figure accordingly.</t>
+  </si>
+  <si>
+    <t>Good point, we used this term a lot without explicitly definining it. Added definition in text.</t>
   </si>
 </sst>
 </file>
@@ -236,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,12 +222,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -265,14 +229,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -589,9 +553,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF6D797-3082-504C-90FD-DD602DAAC2B6}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -599,11 +563,13 @@
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="113.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="47.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -617,7 +583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="409" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -625,33 +591,25 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:6" ht="362" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="280" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="280" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -659,17 +617,17 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="400" x14ac:dyDescent="0.25">
+      <c r="E4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -677,11 +635,11 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="80" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -689,10 +647,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="160" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -700,11 +658,11 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -712,11 +670,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -724,70 +682,52 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>1</v>
-      </c>
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="408" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="409" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
packaging for final coauthor review
</commit_message>
<xml_diff>
--- a/Final Submission/comment_responses_update.xlsx
+++ b/Final Submission/comment_responses_update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gzuckerman/Documents/GitHub/Plasticity1/Final Submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9650ED-9A92-EF4D-8F0A-658005B0E817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37070DAF-C357-504F-A11F-14082708E772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{5D8CA695-E3F1-9847-A2F9-D708B767974E}"/>
+    <workbookView xWindow="-10320" yWindow="-28300" windowWidth="25600" windowHeight="28300" xr2:uid="{5D8CA695-E3F1-9847-A2F9-D708B767974E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>The authors cite Arnold’s (2010) paper about informative parameters in AIC-based model selection, but then perform interpretation on models that contain uninformative parameters. My understanding is that the premise of Arnold (2010) is that if a nested model is within 2 AIC units of a more complex model, then the parameters in the more complex models are uninformative. Here, the authors identify parameters as “informative” when I believe the should not be; for example the top-ranked model in Appendix C contains no informative parameters, since the null model (with no covariates) is within 2 AIC units. </t>
   </si>
@@ -106,15 +106,6 @@
     <t>2. you only need 2 strategies for switching, doesn't matter how many</t>
   </si>
   <si>
-    <t>add this to disucssion: We note that although this is the most comprehensive sample of multiyear elk movement  data from the GYE ecosystem, it is possibleour results under- or oover-estimated switching rates given that we lacked multiple years of conescutive data from 6 of the 26 known herds in the ecosystem</t>
-  </si>
-  <si>
-    <t>could add sentence or two saying that bc of the automated nature of switching identification there could be elk that were in one year on one side of a cluster boundary and in the next, on the other. So there may be some switches that are not bioligically significant, relatively small differences. So we can't say whether all the switches we observed have considerable biolical consequences. We chose this automated apporach bc is it a repeatble objective way to classify behavior whitout predefining behaviors. It is possible that relatively minor shifts in distances traversed or elevation changed, its possibel that a switch may not have strogn bioligcal implications</t>
-  </si>
-  <si>
-    <t>thank you we agree, we have added multiple sentences of discussion. We appreciate this concern as it important to note</t>
-  </si>
-  <si>
     <t>With the way that we performed model selection, whether or not a parameter is informative is not related to how the model compares to the null model - instead it has to do with if the 85% CI overlaps zero. I think what the reviewer may be trying to get at is that there is a "penalty" for a model having more covariates, such that an extra covariate that is uninformative can still result in a model with 2AIC of the top model (see Note). Our top model had more than one parameter different from the next model, thus the fact that it was within 2AIC of the null model is irrelevant.
 We have clarified the text that we used the 85% CI not overlapping 0 as an indicator of a informative parameter. We also added parameter CI ranges in Appendix S3.</t>
   </si>
@@ -122,20 +113,23 @@
     <t>The correlation between switching prevalence and herd migratory diversity was only 0.21, which is quite low. Nearly all (90%) of the herds we studied had more than 1 migratory strategy. In our opinion, if behavioral switching is an important driver of migratory changes, then an elk should be similarly likely to switch between between 2 tactics as between 4 - i.e., the number of possible behavioral tactics matters less than the propensity to change between any tactic. Additionally, the diversity metric is not just a measure of the number of tactics, but the distribution within the herd as well, adding increased nuance to the relationship. With all the above factors considered, we believe there is still significant variation in the data that warrants the modeling we performed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thank you for pointing out that we missed, this--it is a key point. We added a sentence in the methods section clarifying the herd level representation covered by the dataset used in this report. We also added a sentence in the discussion section about this as well. </t>
-  </si>
-  <si>
     <t>This makes sense, we have reordered the figure accordingly.</t>
   </si>
   <si>
     <t>Good point, we used this term a lot without explicitly definining it. Added definition in text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for pointing out that we missed this--it is a key point. We added a sentence in the methods section clarifying the herd level representation covered by the dataset used in this report. We also added a sentence in the discussion section about this as well. </t>
+  </si>
+  <si>
+    <t>Thank you for this key point of feedback. We certainly agree that our automated leaves room for non-biologically consequential switches. We acknowledge this limitation in our discussion section, adding several sentences. Despite the possibility of relatively small changes in behavior being classified as switching, we feel our approach is justified as it is an objective, reproducible methodology that does not rely upon predetermined behaviors. Again, we appreciate you noting this concern.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,31 +161,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,22 +197,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -555,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF6D797-3082-504C-90FD-DD602DAAC2B6}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,6 +545,8 @@
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -591,25 +556,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="362" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="280" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="140" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -620,14 +589,14 @@
         <v>15</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="400" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -638,8 +607,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -649,8 +620,11 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="80" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -661,6 +635,8 @@
         <v>17</v>
       </c>
       <c r="D7" s="1"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -670,9 +646,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -682,40 +660,39 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="12"/>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -728,6 +705,8 @@
         <v>20</v>
       </c>
       <c r="D12" s="1"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
convert comment/responses to word doc
</commit_message>
<xml_diff>
--- a/Final Submission/comment_responses_update.xlsx
+++ b/Final Submission/comment_responses_update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gzuckerman/Documents/GitHub/Plasticity1/Final Submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37070DAF-C357-504F-A11F-14082708E772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCA8A15-1C47-2C4A-8F0A-560CC76EB389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10320" yWindow="-28300" windowWidth="25600" windowHeight="28300" xr2:uid="{5D8CA695-E3F1-9847-A2F9-D708B767974E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>The authors cite Arnold’s (2010) paper about informative parameters in AIC-based model selection, but then perform interpretation on models that contain uninformative parameters. My understanding is that the premise of Arnold (2010) is that if a nested model is within 2 AIC units of a more complex model, then the parameters in the more complex models are uninformative. Here, the authors identify parameters as “informative” when I believe the should not be; for example the top-ranked model in Appendix C contains no informative parameters, since the null model (with no covariates) is within 2 AIC units. </t>
   </si>
@@ -98,12 +98,6 @@
   </si>
   <si>
     <t>We agree that our ability to speak about long-term trends of migratory behavior is limited. We mention this limitation in the second to last paragraph in the Discussion section, but have added to it in accordance with this comment. We have also made sure to specify that the trends we see are during our study period, and may or may not be reflected outside of it. If we do comment on the long term, we make sure to clearly state it is speculation rather than inference from the results</t>
-  </si>
-  <si>
-    <t>between 2 tactics as between 4 - i.e., the number of possible behavioral tactics matters less than the propensity to change between any tactic.</t>
-  </si>
-  <si>
-    <t>2. you only need 2 strategies for switching, doesn't matter how many</t>
   </si>
   <si>
     <t>With the way that we performed model selection, whether or not a parameter is informative is not related to how the model compares to the null model - instead it has to do with if the 85% CI overlaps zero. I think what the reviewer may be trying to get at is that there is a "penalty" for a model having more covariates, such that an extra covariate that is uninformative can still result in a model with 2AIC of the top model (see Note). Our top model had more than one parameter different from the next model, thus the fact that it was within 2AIC of the null model is irrelevant.
@@ -182,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,11 +191,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF6D797-3082-504C-90FD-DD602DAAC2B6}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>14</v>
@@ -572,7 +562,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
@@ -589,12 +579,8 @@
         <v>15</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -646,7 +632,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
@@ -660,7 +646,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
@@ -674,23 +660,23 @@
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="8"/>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>

</xml_diff>